<commit_message>
protein tags sans start stop
</commit_message>
<xml_diff>
--- a/ProteinTags.xlsx
+++ b/ProteinTags.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12220" tabRatio="500"/>
+    <workbookView xWindow="8580" yWindow="1100" windowWidth="28800" windowHeight="12220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -57,34 +57,34 @@
     <t>NES1</t>
   </si>
   <si>
-    <t>atgAAGATTGAAGAAGGTAAGTTGGTTATCTGGATTAACGGTGACAAGGGTTACAACGGTTTGGCTGAAGTTGGTAAGAAATTTGAAAAAGATACCGGTATCAAGGTCACTGTTGAACACCCAGACAAGTTGGAAGAAAAGTTTCCACAAGTTGCTGCCACTGGTGATGGTCCAGACATTATCTTCTGGGCTCATGACAGATTCGGTGGTTACGCCCAATCCGGTTTGTTAGCCGAGATCACCCCAGATAAGGCTTTTCAAGATAAGTTGTATCCATTCACTTGGGATGCCGTCAGATACAACGGTAAGTTAATCGCCTACCCAATTGCTGTTGAAGCTTTGTCTTTGATCTACAATAAGGACTTGTTACCTAACCCACCAAAGACCTGGGAAGAAATCCCAGCTTTAGATAAGGAGTTAAAAGCTAAGGGTAAGTCCGCTTTGATGTTTAACTTGCAAGAACCATACTTCACTTGGCCATTGATCGCTGCTGATGGTGGTTACGCTTTTAAGTATGAAAACGGTAAATACGACATTAAGGATGTCGGTGTCGACAATGCTGGTGCTAAGGCCGGTTTAACTTTCTTAGTCGATTTGATTAAGAATAAACATATGAATGCTGACACTGATTACTCTATTGCTGAAGCTGCTTTCAACAAGGGTGAAACCGCTATGACTATTAACGGTCCATGGGCCTGGTCTAACATTGATACCTCTAAAGTCAACTACGGTGTCACCGTCTTGCCAACTTTTAAGGGTCAACCATCTAAGCCATTCGTCGGTGTCTTGTCTGCCGGTATTAACGCTGCCTCTCCAAATAAGGAATTGGCCAAGGAATTCTTAGAAAACTACTTGTTAACCGATGAAGGTTTAGAGGCCGTTAACAAGGATAAGCCATTAGGTGCTGTTGCTTTGAAGTCTTACGAAGAAGAGTTGGCTAAGGATCCAAGAATTGCTGCTACTATGGAAAACGCTCAAAAGGGTGAAATTATGCCAAACATCCCACAAATGTCTGCTTTCTGGTACGCTGTTCGTACCGCCGTCATTAATGCCGCTTCTGGTCGTCAAACTGTTGATGAAGCCTTGAAGGACGCTCAAACCAGAATTACTAAGtaa</t>
-  </si>
-  <si>
-    <t>ATGtctaaaggtgaagaattattcactggtgttgtcccaattttggttgaattagatggtgatgttaatggtcacaaattttctgtctccggtgaaggtgaaggtgatgctacttacggtaaattgaccttaaaatttatttgtactactggtaaattgccagttccatggccaaccttagtcactactttcggttatggtgttcaatgttttgcgagatacccagatcatatgaaacaacatgactttttcaagtctgccatgccagaaggttatgttcaagaaagaactatttttttcaaagatgacggtaactacaagaccagagctgaagtcaagtttgaaggtgataccttagttaatagaatcgaattaaaaggtattgattttaaagaagatggtaacattttaggtcacaaattggaatacaactataactctcacaatgtttacatcatggctgacaaacaaaagaatggtatcaaagttaacttcaaaattagacacaacattgaagatggttctgttcaattagctgaccattatcaacaaaatactccaattggtgatggtccagtcttgttaccagacaaccattacttatccactcaatctgccttatccaaagatccaaacgaaaagagagaccacatggtcttgttagaatttgttactgctgctggtattatccatggtatggatgaattgtacaaaTAA</t>
-  </si>
-  <si>
-    <t>ATGTCTAAATTATAA</t>
-  </si>
-  <si>
-    <t>ATGtctatggttagtaaaggagaagaaaataacatggcaatcattaaggagttcatgagattcaaagttcacatggaaggttctgtaaatggacatgaatttgaaatagaaggtgaaggagaaggaaggccttatgaaggaacccaaaccgcgaagctaaaagttactaagggtggcccattaccatttgcatgggatatccttagccctcaattcatgtatgggtcaaaggcttatgtcaagcaccccgccgacattccagactatctaaagttatcttttcccgaagggtttaagtgggagcgtgtgatgaacttcgaagacggtggcgtggtaacagtgactcaggattcgtccctgcaagatggtgaatttatctacaaagtcaaattaagaggaactaactttccatctgacggcccggttatgcaaaaaaagacaatgggctgggaggcctcctcagaacgaatgtaccctgaagatggtgccttgaagggtgagattaaacaaagattgaaattgaaagatggtggacattatgacgctgaggttaaaacgacatacaaagctaagaaacctgtccagctcccaggtgcttacaatgtaaatataaaacttgatattacatcacataatgaagattatacgatagttgaacaatacgaaagggctgaggggagacatagtactggtggcatggatgaactatacaaaTAA</t>
-  </si>
-  <si>
-    <t>ATGCTTTCACTACGTCAATCTATAAGATTTTTCAAGCCAGCCACAAGAACTTTGTGTAGCTCTAGATAA</t>
-  </si>
-  <si>
-    <t>ATGGCTTCAGAAAAAGAAATTAGGAGAGAGAGATTCTTGAACGTTTTCCCTAAATTAGTAGAGGAATTGAACGCATCGCTTTTGGCTTACGGTATGCCTAAGGAAGCATGTGACTGGTATGCCCACTCATTGAACTACAACACTCCAGGCGGTAAGCTAAATAGAGGTTTGTCCGTTGTGGACACGTATGCTATTCTCTCCAACAAGACCGTTGAACAATTGGGGCAAGAAGAATACGAAAAGGTTGCCATTCTAGGTTGGTGCATTGAGTTGTTGCAGGCTTACTTCTTGGTCGCCGATGATATGATGGACAAGTCCATTACCAGAAGAGGCCAACCATGTTGGTACAAGGTTCCTGAAGTTGGGGAAATTGCCATCAATGACGCATTCATGTTAGAGGCTGCTATCTACAAGCTTTTGAAATCTCACTTCAGAAACGAAAAATACTACATAGATATCACCGAATTGTTCCATGAGGTCACCTTCCAAACCGAATTGGGCCAATTGATGGACTTAATCACTGCACCTGAAGACAAAGTCGACTTGAGTAAGTTCTCCCTAAAGAAGCACTCCTTCATAGTTACTTTCAAGACTGCTTACTATTCTTTCTACTTGCCTGTCGCATTGGCCATGTACGTTGCCGGTATCACGGATGAAAAGGATTTGAAACAAGCCAGAGATGTCTTGATTCCATTGGGTGAATACTTCCAAATTCAAGATGACTACTTAGACTGCTTCGGTACCCCAGAACAGATCGGTAAGATCGGTACAGATATCCAAGATAACAAATGTTCTTGGGTAATCAACAAGGCATTGGAACTTGCTTCCGCAGAACAAAGAAAGACTTTAGACGAAAATTACGGTAAGAAGGACTCAGTCGCAGAAGCCAAATGCAAAAAGATTTTCAATGACTTGAAAATTGAACAGCTATACCACGAATATGAAGAGTCTATTGCCAAGGATTTGAAGGCCAAAATTTCTCAGGTCGATGAGTCTCGTGGCTTCAAAGCTGATGTCTTAACTGCGTTCTTGAACAAAGTTTACAAGAGAAGCAAATAA</t>
-  </si>
-  <si>
-    <t>ATGCAGATTTTCGTCAAGACTTTGACCGGTAAAACCATAACATTGGAAGTTGAATCTTCCGATACCATCGACAACGTTAAGTCGAAAATTCAAGACAAGGAAGGTATCCCTCCAGATCAACAAAGATTGATCTTTGCCGGTAAGCAGCTAGAAGACGGTAGAACGCTGTCTGATTACAACATTCAGAAGGAGTCCACCTTACATCTTGTGCTAAGGCTAAGAGGTGGTTATCACGGATCCGGAGCTTGGCTGTTGCCCGTCTCACTGGTGAAAAGAAAAACCACCCTGGCGCCCAATACGTAA</t>
-  </si>
-  <si>
-    <t>ATGTCTACCTCTGAAAACCAAAGTAAAGGTAGTGGTACATTGGTTGTCATATTGGCCATTTTAATGCTAGGTGTTGCTTATTATTTGTTGAACGAATAA</t>
-  </si>
-  <si>
-    <t>ATGTGGTACAAGGATCTAAAAATGAAGATGTGTCTGGCTTTAGTAATCATCATATTGCTTGTTGTAATCATCGTCCCCATTGCTGTTCACTTTAGTCGATAA</t>
-  </si>
-  <si>
-    <t>ATGaacgagctggccctgaagctggccggactggacatcTAA</t>
+    <t>TCTAAATTA</t>
+  </si>
+  <si>
+    <t>tctatggttagtaaaggagaagaaaataacatggcaatcattaaggagttcatgagattcaaagttcacatggaaggttctgtaaatggacatgaatttgaaatagaaggtgaaggagaaggaaggccttatgaaggaacccaaaccgcgaagctaaaagttactaagggtggcccattaccatttgcatgggatatccttagccctcaattcatgtatgggtcaaaggcttatgtcaagcaccccgccgacattccagactatctaaagttatcttttcccgaagggtttaagtgggagcgtgtgatgaacttcgaagacggtggcgtggtaacagtgactcaggattcgtccctgcaagatggtgaatttatctacaaagtcaaattaagaggaactaactttccatctgacggcccggttatgcaaaaaaagacaatgggctgggaggcctcctcagaacgaatgtaccctgaagatggtgccttgaagggtgagattaaacaaagattgaaattgaaagatggtggacattatgacgctgaggttaaaacgacatacaaagctaagaaacctgtccagctcccaggtgcttacaatgtaaatataaaacttgatattacatcacataatgaagattatacgatagttgaacaatacgaaagggctgaggggagacatagtactggtggcatggatgaactatacaaa</t>
+  </si>
+  <si>
+    <t>AAGATTGAAGAAGGTAAGTTGGTTATCTGGATTAACGGTGACAAGGGTTACAACGGTTTGGCTGAAGTTGGTAAGAAATTTGAAAAAGATACCGGTATCAAGGTCACTGTTGAACACCCAGACAAGTTGGAAGAAAAGTTTCCACAAGTTGCTGCCACTGGTGATGGTCCAGACATTATCTTCTGGGCTCATGACAGATTCGGTGGTTACGCCCAATCCGGTTTGTTAGCCGAGATCACCCCAGATAAGGCTTTTCAAGATAAGTTGTATCCATTCACTTGGGATGCCGTCAGATACAACGGTAAGTTAATCGCCTACCCAATTGCTGTTGAAGCTTTGTCTTTGATCTACAATAAGGACTTGTTACCTAACCCACCAAAGACCTGGGAAGAAATCCCAGCTTTAGATAAGGAGTTAAAAGCTAAGGGTAAGTCCGCTTTGATGTTTAACTTGCAAGAACCATACTTCACTTGGCCATTGATCGCTGCTGATGGTGGTTACGCTTTTAAGTATGAAAACGGTAAATACGACATTAAGGATGTCGGTGTCGACAATGCTGGTGCTAAGGCCGGTTTAACTTTCTTAGTCGATTTGATTAAGAATAAACATATGAATGCTGACACTGATTACTCTATTGCTGAAGCTGCTTTCAACAAGGGTGAAACCGCTATGACTATTAACGGTCCATGGGCCTGGTCTAACATTGATACCTCTAAAGTCAACTACGGTGTCACCGTCTTGCCAACTTTTAAGGGTCAACCATCTAAGCCATTCGTCGGTGTCTTGTCTGCCGGTATTAACGCTGCCTCTCCAAATAAGGAATTGGCCAAGGAATTCTTAGAAAACTACTTGTTAACCGATGAAGGTTTAGAGGCCGTTAACAAGGATAAGCCATTAGGTGCTGTTGCTTTGAAGTCTTACGAAGAAGAGTTGGCTAAGGATCCAAGAATTGCTGCTACTATGGAAAACGCTCAAAAGGGTGAAATTATGCCAAACATCCCACAAATGTCTGCTTTCTGGTACGCTGTTCGTACCGCCGTCATTAATGCCGCTTCTGGTCGTCAAACTGTTGATGAAGCCTTGAAGGACGCTCAAACCAGAATTACTAAG</t>
+  </si>
+  <si>
+    <t>tctaaaggtgaagaattattcactggtgttgtcccaattttggttgaattagatggtgatgttaatggtcacaaattttctgtctccggtgaaggtgaaggtgatgctacttacggtaaattgaccttaaaatttatttgtactactggtaaattgccagttccatggccaaccttagtcactactttcggttatggtgttcaatgttttgcgagatacccagatcatatgaaacaacatgactttttcaagtctgccatgccagaaggttatgttcaagaaagaactatttttttcaaagatgacggtaactacaagaccagagctgaagtcaagtttgaaggtgataccttagttaatagaatcgaattaaaaggtattgattttaaagaagatggtaacattttaggtcacaaattggaatacaactataactctcacaatgtttacatcatggctgacaaacaaaagaatggtatcaaagttaacttcaaaattagacacaacattgaagatggttctgttcaattagctgaccattatcaacaaaatactccaattggtgatggtccagtcttgttaccagacaaccattacttatccactcaatctgccttatccaaagatccaaacgaaaagagagaccacatggtcttgttagaatttgttactgctgctggtattatccatggtatggatgaattgtacaaa</t>
+  </si>
+  <si>
+    <t>CTTTCACTACGTCAATCTATAAGATTTTTCAAGCCAGCCACAAGAACTTTGTGTAGCTCTAGA</t>
+  </si>
+  <si>
+    <t>GCTTCAGAAAAAGAAATTAGGAGAGAGAGATTCTTGAACGTTTTCCCTAAATTAGTAGAGGAATTGAACGCATCGCTTTTGGCTTACGGTATGCCTAAGGAAGCATGTGACTGGTATGCCCACTCATTGAACTACAACACTCCAGGCGGTAAGCTAAATAGAGGTTTGTCCGTTGTGGACACGTATGCTATTCTCTCCAACAAGACCGTTGAACAATTGGGGCAAGAAGAATACGAAAAGGTTGCCATTCTAGGTTGGTGCATTGAGTTGTTGCAGGCTTACTTCTTGGTCGCCGATGATATGATGGACAAGTCCATTACCAGAAGAGGCCAACCATGTTGGTACAAGGTTCCTGAAGTTGGGGAAATTGCCATCAATGACGCATTCATGTTAGAGGCTGCTATCTACAAGCTTTTGAAATCTCACTTCAGAAACGAAAAATACTACATAGATATCACCGAATTGTTCCATGAGGTCACCTTCCAAACCGAATTGGGCCAATTGATGGACTTAATCACTGCACCTGAAGACAAAGTCGACTTGAGTAAGTTCTCCCTAAAGAAGCACTCCTTCATAGTTACTTTCAAGACTGCTTACTATTCTTTCTACTTGCCTGTCGCATTGGCCATGTACGTTGCCGGTATCACGGATGAAAAGGATTTGAAACAAGCCAGAGATGTCTTGATTCCATTGGGTGAATACTTCCAAATTCAAGATGACTACTTAGACTGCTTCGGTACCCCAGAACAGATCGGTAAGATCGGTACAGATATCCAAGATAACAAATGTTCTTGGGTAATCAACAAGGCATTGGAACTTGCTTCCGCAGAACAAAGAAAGACTTTAGACGAAAATTACGGTAAGAAGGACTCAGTCGCAGAAGCCAAATGCAAAAAGATTTTCAATGACTTGAAAATTGAACAGCTATACCACGAATATGAAGAGTCTATTGCCAAGGATTTGAAGGCCAAAATTTCTCAGGTCGATGAGTCTCGTGGCTTCAAAGCTGATGTCTTAACTGCGTTCTTGAACAAAGTTTACAAGAGAAGCAAA</t>
+  </si>
+  <si>
+    <t>CAGATTTTCGTCAAGACTTTGACCGGTAAAACCATAACATTGGAAGTTGAATCTTCCGATACCATCGACAACGTTAAGTCGAAAATTCAAGACAAGGAAGGTATCCCTCCAGATCAACAAAGATTGATCTTTGCCGGTAAGCAGCTAGAAGACGGTAGAACGCTGTCTGATTACAACATTCAGAAGGAGTCCACCTTACATCTTGTGCTAAGGCTAAGAGGTGGTTATCACGGATCCGGAGCTTGGCTGTTGCCCGTCTCACTGGTGAAAAGAAAAACCACCCTGGCGCCCAATACG</t>
+  </si>
+  <si>
+    <t>TCTACCTCTGAAAACCAAAGTAAAGGTAGTGGTACATTGGTTGTCATATTGGCCATTTTAATGCTAGGTGTTGCTTATTATTTGTTGAACGAA</t>
+  </si>
+  <si>
+    <t>TGGTACAAGGATCTAAAAATGAAGATGTGTCTGGCTTTAGTAATCATCATATTGCTTGTTGTAATCATCGTCCCCATTGCTGTTCACTTTAGTCGA</t>
+  </si>
+  <si>
+    <t>aacgagctggccctgaagctggccggactggacatc</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -543,7 +543,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -551,7 +551,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -559,7 +559,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">

</xml_diff>

<commit_message>
protein tags and manual
</commit_message>
<xml_diff>
--- a/ProteinTags.xlsx
+++ b/ProteinTags.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leodespaux/Google Drive/Code/CASdesigner/CASdesigner-web/casdesigner-web/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="1100" windowWidth="28800" windowHeight="12220" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>MBP</t>
   </si>
@@ -39,21 +47,12 @@
     <t>mCherry</t>
   </si>
   <si>
-    <t>COX4</t>
-  </si>
-  <si>
     <t>ERG20</t>
   </si>
   <si>
     <t>UbiX</t>
   </si>
   <si>
-    <t>CYB5</t>
-  </si>
-  <si>
-    <t>SNC1</t>
-  </si>
-  <si>
     <t>NES1</t>
   </si>
   <si>
@@ -85,6 +84,27 @@
   </si>
   <si>
     <t>aacgagctggccctgaagctggccggactggacatc</t>
+  </si>
+  <si>
+    <t>MT1</t>
+  </si>
+  <si>
+    <t>ER1</t>
+  </si>
+  <si>
+    <t>ER2</t>
+  </si>
+  <si>
+    <t>PM1</t>
+  </si>
+  <si>
+    <t>ATATTAGAGCAACCTCTGAAAT TTGTGCTTACTGCGGCCGTCGTG CTCTTGACGACGTCGGTTCTTTG TTGTGTAGTATTTACA</t>
+  </si>
+  <si>
+    <t>AATATAAAAGAAATAATGTGGT GGCAGAAGGTCAAAAATATTAC GTTATTAACTTTCACTATTATAC TATTTGTAAGTGCTGCTTTCATG TTTTTCTATCTGTGG</t>
+  </si>
+  <si>
+    <t>VC1</t>
   </si>
 </sst>
 </file>
@@ -97,7 +117,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -145,9 +164,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -163,17 +194,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -511,18 +554,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A2" sqref="A2:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -530,93 +573,104 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>